<commit_message>
Google Translation and ReadWrite Excel Updated
</commit_message>
<xml_diff>
--- a/MRTK_Content.xlsx
+++ b/MRTK_Content.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23921"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37619451-18A1-4890-88B1-08D28E3C05FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5A605A5-D996-4745-97CD-A6DC1A76E621}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="394">
   <si>
     <t>Topic
 トピック</t>
@@ -53,23 +53,6 @@
   <si>
     <t>Welcome To MRTK
 MRTKへようこそ</t>
-  </si>
-  <si>
-    <t>Getting started with MRTK
-Documentation
-Build status
-Feature areas
-UX building blocks
-Tools
-Example scenes
-MRTK examples hub
-Sample apps made with MRTK
-Session videos from Mixed Reality Dev Days 2020
-Engage with the community
-Useful resources on the Mixed Reality Dev Center
-Useful resources on Azure
-How to contribute
-Getting help</t>
   </si>
   <si>
     <t>Getting started with MRTK
@@ -1763,7 +1746,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1783,13 +1766,6 @@
       <b/>
       <sz val="18"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1869,7 +1845,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1955,11 +1931,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2301,10 +2276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G155"/>
+  <dimension ref="A1:F155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B51" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2313,12 +2288,11 @@
     <col min="2" max="2" width="48" style="2" customWidth="1"/>
     <col min="3" max="3" width="61.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="66.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="170.42578125" customWidth="1"/>
+    <col min="5" max="5" width="66.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="170.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="64.5" customHeight="1">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="64.5" customHeight="1">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -2331,2329 +2305,2172 @@
       <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="24" customFormat="1" ht="409.5" customHeight="1">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:6" s="24" customFormat="1" ht="409.5" customHeight="1">
+      <c r="A2" s="37" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="39" t="s">
+    </row>
+    <row r="3" spans="1:6" s="10" customFormat="1" ht="45" customHeight="1">
+      <c r="A3" s="39" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="10" customFormat="1" ht="45" customHeight="1">
-      <c r="A3" s="40" t="s">
-        <v>10</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" s="10" customFormat="1" ht="131.25" customHeight="1">
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" s="10" customFormat="1" ht="131.25" customHeight="1">
       <c r="A4" s="6"/>
       <c r="B4" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="16"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="17" t="s">
+      <c r="E4" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="41" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="10" customFormat="1" ht="200.25" customHeight="1">
+    </row>
+    <row r="5" spans="1:6" s="10" customFormat="1" ht="200.25" customHeight="1">
       <c r="A5" s="6"/>
       <c r="B5" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="16"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="17" t="s">
+      <c r="E5" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="41" t="s">
+    </row>
+    <row r="6" spans="1:6" s="24" customFormat="1" ht="109.5" customHeight="1">
+      <c r="A6" s="37" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="24" customFormat="1" ht="109.5" customHeight="1">
-      <c r="A6" s="38" t="s">
-        <v>17</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="23"/>
       <c r="D6" s="22"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="21" t="s">
+      <c r="E6" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="39" t="s">
+    </row>
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="30" customHeight="1">
+      <c r="A7" s="41" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="10" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="42" t="s">
-        <v>20</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" s="10" customFormat="1" ht="98.25" customHeight="1">
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" s="10" customFormat="1" ht="98.25" customHeight="1">
       <c r="A8" s="11"/>
-      <c r="B8" s="43" t="s">
-        <v>21</v>
+      <c r="B8" s="42" t="s">
+        <v>20</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="16"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="17" t="s">
+      <c r="E8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="18" t="s">
+    </row>
+    <row r="9" spans="1:6" s="10" customFormat="1" ht="159" customHeight="1">
+      <c r="A9" s="11"/>
+      <c r="B9" s="42" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="10" customFormat="1" ht="159" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="43" t="s">
-        <v>24</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="17" t="s">
+      <c r="E9" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="18" t="s">
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="108.75" customHeight="1">
+      <c r="A10" s="11"/>
+      <c r="B10" s="42" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="10" customFormat="1" ht="108.75" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="43" t="s">
-        <v>27</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="17" t="s">
+      <c r="E10" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="18" t="s">
+    </row>
+    <row r="11" spans="1:6" s="13" customFormat="1" ht="408" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="42" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="13" customFormat="1" ht="408" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="43" t="s">
-        <v>30</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="15" t="s">
+      <c r="E11" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="44" t="s">
+    </row>
+    <row r="12" spans="1:6" s="24" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A12" s="44" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="24" customFormat="1" ht="42" customHeight="1">
-      <c r="A12" s="45" t="s">
-        <v>33</v>
       </c>
       <c r="B12" s="26"/>
       <c r="C12" s="21"/>
       <c r="D12" s="22"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="25"/>
-    </row>
-    <row r="13" spans="1:7" s="24" customFormat="1" ht="78" customHeight="1">
+      <c r="E12" s="22"/>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="1:6" s="24" customFormat="1" ht="78" customHeight="1">
       <c r="A13" s="26"/>
       <c r="B13" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="29"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="28" t="s">
+      <c r="E13" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="24" customFormat="1" ht="234" customHeight="1">
+    </row>
+    <row r="14" spans="1:6" s="24" customFormat="1" ht="234" customHeight="1">
       <c r="A14" s="26"/>
       <c r="B14" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="28" t="s">
+      <c r="E14" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="24" customFormat="1" ht="39" customHeight="1">
+    </row>
+    <row r="15" spans="1:6" s="24" customFormat="1" ht="39" customHeight="1">
       <c r="A15" s="26"/>
       <c r="B15" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="28"/>
       <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="24" customFormat="1" ht="256.5" customHeight="1">
+      <c r="E15" s="29"/>
+      <c r="F15" s="31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="24" customFormat="1" ht="256.5" customHeight="1">
       <c r="A16" s="26"/>
       <c r="B16" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="29"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="28" t="s">
+      <c r="E16" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="31" t="s">
+    </row>
+    <row r="17" spans="1:6" s="10" customFormat="1" ht="30">
+      <c r="A17" s="41" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="10" customFormat="1" ht="30">
-      <c r="A17" s="42" t="s">
-        <v>45</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="12"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" s="10" customFormat="1" ht="60">
+      <c r="E17" s="8"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" s="10" customFormat="1" ht="60">
       <c r="A18" s="11"/>
-      <c r="B18" s="43" t="s">
-        <v>46</v>
+      <c r="B18" s="42" t="s">
+        <v>45</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="16"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="18" t="s">
+    </row>
+    <row r="19" spans="1:6" s="10" customFormat="1" ht="136.5" customHeight="1">
+      <c r="A19" s="11"/>
+      <c r="B19" s="42" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="10" customFormat="1" ht="136.5" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="43" t="s">
-        <v>49</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="17" t="s">
+      <c r="E19" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="18" t="s">
+    </row>
+    <row r="20" spans="1:6" s="24" customFormat="1" ht="54" customHeight="1">
+      <c r="A20" s="44" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="24" customFormat="1" ht="54" customHeight="1">
-      <c r="A20" s="45" t="s">
-        <v>52</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="21"/>
       <c r="D20" s="22"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="25"/>
-    </row>
-    <row r="21" spans="1:7" s="24" customFormat="1" ht="132" customHeight="1">
+      <c r="E20" s="22"/>
+      <c r="F20" s="25"/>
+    </row>
+    <row r="21" spans="1:6" s="24" customFormat="1" ht="132" customHeight="1">
       <c r="A21" s="26"/>
       <c r="B21" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="28"/>
       <c r="D21" s="29"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="28" t="s">
+      <c r="E21" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G21" s="31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="24" customFormat="1" ht="99" customHeight="1">
+    </row>
+    <row r="22" spans="1:6" s="24" customFormat="1" ht="99" customHeight="1">
       <c r="A22" s="26"/>
       <c r="B22" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="29"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="28" t="s">
+      <c r="E22" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="G22" s="31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="24" customFormat="1" ht="98.25" customHeight="1">
+    </row>
+    <row r="23" spans="1:6" s="24" customFormat="1" ht="98.25" customHeight="1">
       <c r="A23" s="26"/>
       <c r="B23" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="29"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="28" t="s">
+      <c r="E23" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="G23" s="31" t="s">
+    </row>
+    <row r="24" spans="1:6" s="10" customFormat="1" ht="30">
+      <c r="A24" s="41" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="10" customFormat="1" ht="30">
-      <c r="A24" s="42" t="s">
-        <v>62</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="1:7" s="10" customFormat="1" ht="60">
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" spans="1:6" s="10" customFormat="1" ht="60">
       <c r="A25" s="11"/>
-      <c r="B25" s="43" t="s">
-        <v>63</v>
+      <c r="B25" s="42" t="s">
+        <v>62</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="17" t="s">
+      <c r="E25" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G25" s="18" t="s">
+    </row>
+    <row r="26" spans="1:6" s="10" customFormat="1" ht="60">
+      <c r="A26" s="11"/>
+      <c r="B26" s="42" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="10" customFormat="1" ht="60">
-      <c r="A26" s="11"/>
-      <c r="B26" s="43" t="s">
-        <v>66</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="17" t="s">
+      <c r="E26" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G26" s="18" t="s">
+    </row>
+    <row r="27" spans="1:6" s="10" customFormat="1" ht="30">
+      <c r="A27" s="11"/>
+      <c r="B27" s="42" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="10" customFormat="1" ht="30">
-      <c r="A27" s="11"/>
-      <c r="B27" s="43" t="s">
-        <v>69</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="16"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" s="10" customFormat="1" ht="30">
+      <c r="E27" s="16"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" s="10" customFormat="1" ht="30">
       <c r="A28" s="11"/>
       <c r="B28" s="14"/>
       <c r="C28" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="10" customFormat="1" ht="30">
+    </row>
+    <row r="29" spans="1:6" s="10" customFormat="1" ht="30">
       <c r="A29" s="11"/>
       <c r="B29" s="14"/>
       <c r="C29" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="18" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="10" customFormat="1" ht="90">
+    </row>
+    <row r="30" spans="1:6" s="10" customFormat="1" ht="90">
       <c r="A30" s="11"/>
       <c r="B30" s="14"/>
       <c r="C30" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="17" t="s">
+      <c r="F30" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="G30" s="18" t="s">
+    </row>
+    <row r="31" spans="1:6" s="10" customFormat="1" ht="90">
+      <c r="A31" s="11"/>
+      <c r="B31" s="42" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="10" customFormat="1" ht="90">
-      <c r="A31" s="11"/>
-      <c r="B31" s="43" t="s">
-        <v>77</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="16"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="17" t="s">
+      <c r="E31" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="G31" s="18" t="s">
+    </row>
+    <row r="32" spans="1:6" s="24" customFormat="1" ht="30">
+      <c r="A32" s="44" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="24" customFormat="1" ht="30">
-      <c r="A32" s="45" t="s">
-        <v>80</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="21"/>
       <c r="D32" s="22"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="25"/>
-    </row>
-    <row r="33" spans="1:7" s="24" customFormat="1" ht="30">
+      <c r="E32" s="22"/>
+      <c r="F32" s="25"/>
+    </row>
+    <row r="33" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A33" s="26"/>
       <c r="B33" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="28"/>
       <c r="D33" s="29"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
-    </row>
-    <row r="34" spans="1:7" s="24" customFormat="1" ht="150">
+      <c r="E33" s="29"/>
+      <c r="F33" s="30"/>
+    </row>
+    <row r="34" spans="1:6" s="24" customFormat="1" ht="150">
       <c r="A34" s="26"/>
       <c r="B34" s="27"/>
       <c r="C34" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="29"/>
+      <c r="E34" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="28" t="s">
+      <c r="F34" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="G34" s="31" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" s="24" customFormat="1" ht="180">
+    </row>
+    <row r="35" spans="1:6" s="24" customFormat="1" ht="180">
       <c r="A35" s="26"/>
       <c r="B35" s="27"/>
       <c r="C35" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="28" t="s">
+      <c r="F35" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="G35" s="31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="36" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A36" s="26"/>
       <c r="B36" s="32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C36" s="28"/>
       <c r="D36" s="29"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="30"/>
-    </row>
-    <row r="37" spans="1:7" s="24" customFormat="1" ht="60">
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
+    </row>
+    <row r="37" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A37" s="26"/>
       <c r="B37" s="27"/>
       <c r="C37" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="29"/>
+      <c r="E37" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="28" t="s">
+      <c r="F37" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="G37" s="31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="38" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A38" s="26"/>
       <c r="B38" s="27"/>
       <c r="C38" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="29"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="D38" s="29"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="39" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A39" s="26"/>
       <c r="B39" s="27"/>
       <c r="C39" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="29"/>
+      <c r="E39" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D39" s="29"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="28" t="s">
+      <c r="F39" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="G39" s="31" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="40" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A40" s="26"/>
       <c r="B40" s="27"/>
       <c r="C40" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="29"/>
+      <c r="E40" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="D40" s="29"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="28" t="s">
+      <c r="F40" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="G40" s="31" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="41" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A41" s="26"/>
       <c r="B41" s="32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C41" s="28"/>
       <c r="D41" s="29"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="30"/>
-    </row>
-    <row r="42" spans="1:7" s="24" customFormat="1" ht="30">
+      <c r="E41" s="29"/>
+      <c r="F41" s="30"/>
+    </row>
+    <row r="42" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A42" s="26"/>
       <c r="B42" s="27"/>
       <c r="C42" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="29"/>
+      <c r="E42" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="29"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="28" t="s">
+      <c r="F42" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="G42" s="31" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="24" customFormat="1" ht="180">
+    </row>
+    <row r="43" spans="1:6" s="24" customFormat="1" ht="180">
       <c r="A43" s="26"/>
       <c r="B43" s="27"/>
       <c r="C43" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D43" s="29"/>
+      <c r="E43" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="D43" s="29"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="28" t="s">
+      <c r="F43" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="G43" s="31" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="24" customFormat="1" ht="270">
+    </row>
+    <row r="44" spans="1:6" s="24" customFormat="1" ht="270">
       <c r="A44" s="26"/>
       <c r="B44" s="27"/>
       <c r="C44" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="29"/>
+      <c r="E44" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="28" t="s">
+      <c r="F44" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="G44" s="31" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="24" customFormat="1" ht="90">
+    </row>
+    <row r="45" spans="1:6" s="24" customFormat="1" ht="90">
       <c r="A45" s="26"/>
       <c r="B45" s="27"/>
       <c r="C45" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="29"/>
+      <c r="E45" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="D45" s="29"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="28" t="s">
+      <c r="F45" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G45" s="31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="46" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A46" s="26"/>
       <c r="B46" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C46" s="28"/>
       <c r="D46" s="29"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="30"/>
-    </row>
-    <row r="47" spans="1:7" s="24" customFormat="1" ht="90">
+      <c r="E46" s="29"/>
+      <c r="F46" s="30"/>
+    </row>
+    <row r="47" spans="1:6" s="24" customFormat="1" ht="90">
       <c r="A47" s="26"/>
       <c r="B47" s="27"/>
       <c r="C47" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D47" s="29"/>
+      <c r="E47" s="28" t="s">
         <v>114</v>
       </c>
-      <c r="D47" s="29"/>
-      <c r="E47" s="30"/>
-      <c r="F47" s="28" t="s">
+      <c r="F47" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="G47" s="31" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="48" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A48" s="26"/>
       <c r="B48" s="27"/>
       <c r="C48" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="29"/>
+      <c r="E48" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="D48" s="29"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="28" t="s">
+      <c r="F48" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="G48" s="31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="49" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A49" s="26"/>
       <c r="B49" s="27"/>
       <c r="C49" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D49" s="29"/>
+      <c r="E49" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="D49" s="29"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="28" t="s">
+      <c r="F49" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="G49" s="31" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="50" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A50" s="26"/>
       <c r="B50" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C50" s="28"/>
       <c r="D50" s="29"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="30"/>
-    </row>
-    <row r="51" spans="1:7" s="24" customFormat="1" ht="180">
+      <c r="E50" s="29"/>
+      <c r="F50" s="30"/>
+    </row>
+    <row r="51" spans="1:6" s="24" customFormat="1" ht="180">
       <c r="A51" s="26"/>
       <c r="B51" s="27"/>
       <c r="C51" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" s="29"/>
+      <c r="E51" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="D51" s="29"/>
-      <c r="E51" s="30"/>
-      <c r="F51" s="28" t="s">
+      <c r="F51" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="G51" s="31" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" s="24" customFormat="1" ht="150">
+    </row>
+    <row r="52" spans="1:6" s="24" customFormat="1" ht="150">
       <c r="A52" s="26"/>
       <c r="B52" s="27"/>
       <c r="C52" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D52" s="29"/>
+      <c r="E52" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="D52" s="29"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="28" t="s">
+      <c r="F52" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="G52" s="31" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="53" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A53" s="26"/>
       <c r="B53" s="27"/>
       <c r="C53" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" s="29"/>
+      <c r="E53" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="D53" s="29"/>
-      <c r="E53" s="30"/>
-      <c r="F53" s="28" t="s">
+      <c r="F53" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="G53" s="31" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="54" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A54" s="26"/>
       <c r="B54" s="27"/>
       <c r="C54" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D54" s="29"/>
+      <c r="E54" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="29"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="28" t="s">
+      <c r="F54" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="G54" s="31" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="55" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A55" s="26"/>
       <c r="B55" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C55" s="28"/>
       <c r="D55" s="29"/>
-      <c r="E55" s="30"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="30"/>
-    </row>
-    <row r="56" spans="1:7" s="24" customFormat="1" ht="45">
+      <c r="E55" s="29"/>
+      <c r="F55" s="30"/>
+    </row>
+    <row r="56" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A56" s="26"/>
       <c r="B56" s="27"/>
       <c r="C56" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" s="29"/>
+      <c r="E56" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D56" s="29"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="28" t="s">
+      <c r="F56" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="G56" s="31" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="57" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A57" s="26"/>
       <c r="B57" s="27"/>
       <c r="C57" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="D57" s="29"/>
+      <c r="E57" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="D57" s="29"/>
-      <c r="E57" s="30"/>
-      <c r="F57" s="28" t="s">
+      <c r="F57" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="G57" s="31" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" s="24" customFormat="1" ht="90">
+    </row>
+    <row r="58" spans="1:6" s="24" customFormat="1" ht="90">
       <c r="A58" s="26"/>
       <c r="B58" s="27"/>
       <c r="C58" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D58" s="29"/>
+      <c r="E58" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="D58" s="29"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="28" t="s">
+      <c r="F58" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="G58" s="31" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="59" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A59" s="26"/>
       <c r="B59" s="27"/>
       <c r="C59" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="D59" s="29"/>
+      <c r="E59" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="D59" s="29"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="28" t="s">
+      <c r="F59" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="G59" s="31" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="60" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A60" s="26"/>
       <c r="B60" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C60" s="28"/>
       <c r="D60" s="29"/>
-      <c r="E60" s="30"/>
-      <c r="F60" s="29"/>
-      <c r="G60" s="30"/>
-    </row>
-    <row r="61" spans="1:7" s="24" customFormat="1" ht="45">
+      <c r="E60" s="29"/>
+      <c r="F60" s="30"/>
+    </row>
+    <row r="61" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A61" s="26"/>
       <c r="B61" s="27"/>
       <c r="C61" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D61" s="29"/>
+      <c r="E61" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="D61" s="29"/>
-      <c r="E61" s="30"/>
-      <c r="F61" s="28" t="s">
+      <c r="F61" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="G61" s="31" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="62" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A62" s="26"/>
       <c r="B62" s="27"/>
       <c r="C62" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D62" s="29"/>
-      <c r="E62" s="30"/>
-      <c r="F62" s="28" t="s">
+      <c r="E62" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F62" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="G62" s="31" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="63" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A63" s="26"/>
       <c r="B63" s="27"/>
       <c r="C63" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="D63" s="29"/>
+      <c r="E63" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="D63" s="29"/>
-      <c r="E63" s="30"/>
-      <c r="F63" s="28" t="s">
+      <c r="F63" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="G63" s="31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="64" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A64" s="26"/>
       <c r="B64" s="27"/>
       <c r="C64" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="D64" s="29"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="29" t="s">
+      <c r="F64" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="G64" s="31" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="65" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A65" s="26"/>
       <c r="B65" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C65" s="28"/>
       <c r="D65" s="29"/>
-      <c r="E65" s="30"/>
-      <c r="F65" s="29"/>
-      <c r="G65" s="30"/>
-    </row>
-    <row r="66" spans="1:7" s="24" customFormat="1" ht="30">
+      <c r="E65" s="29"/>
+      <c r="F65" s="30"/>
+    </row>
+    <row r="66" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A66" s="26"/>
       <c r="B66" s="27"/>
       <c r="C66" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="D66" s="29"/>
-      <c r="E66" s="30"/>
-      <c r="F66" s="29"/>
-      <c r="G66" s="31" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" s="24" customFormat="1" ht="90">
+    </row>
+    <row r="67" spans="1:6" s="24" customFormat="1" ht="90">
       <c r="A67" s="26"/>
       <c r="B67" s="27"/>
       <c r="C67" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="D67" s="29"/>
+      <c r="E67" s="28" t="s">
         <v>164</v>
       </c>
-      <c r="D67" s="29"/>
-      <c r="E67" s="30"/>
-      <c r="F67" s="28" t="s">
+      <c r="F67" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="G67" s="31" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="68" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A68" s="26"/>
       <c r="B68" s="27"/>
       <c r="C68" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="D68" s="29"/>
+      <c r="E68" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="D68" s="29"/>
-      <c r="E68" s="30"/>
-      <c r="F68" s="28" t="s">
+      <c r="F68" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="G68" s="31" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="69" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A69" s="26"/>
       <c r="B69" s="27"/>
       <c r="C69" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="D69" s="29"/>
+      <c r="E69" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="D69" s="29"/>
-      <c r="E69" s="30"/>
-      <c r="F69" s="28" t="s">
+      <c r="F69" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="G69" s="31" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="70" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A70" s="26"/>
       <c r="B70" s="27"/>
       <c r="C70" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="D70" s="29"/>
+      <c r="E70" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="D70" s="29"/>
-      <c r="E70" s="30"/>
-      <c r="F70" s="28" t="s">
+      <c r="F70" s="31" t="s">
         <v>174</v>
       </c>
-      <c r="G70" s="31" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" s="24" customFormat="1" ht="90">
+    </row>
+    <row r="71" spans="1:6" s="24" customFormat="1" ht="90">
       <c r="A71" s="26"/>
       <c r="B71" s="27"/>
       <c r="C71" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="D71" s="29"/>
+      <c r="E71" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="D71" s="29"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="28" t="s">
+      <c r="F71" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="G71" s="31" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="72" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A72" s="26"/>
       <c r="B72" s="27"/>
       <c r="C72" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="D72" s="29"/>
+      <c r="E72" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="D72" s="29"/>
-      <c r="E72" s="30"/>
-      <c r="F72" s="28" t="s">
+      <c r="F72" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="G72" s="31" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="73" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A73" s="26"/>
       <c r="B73" s="27"/>
       <c r="C73" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="D73" s="29"/>
+      <c r="E73" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="D73" s="29"/>
-      <c r="E73" s="30"/>
-      <c r="F73" s="28" t="s">
+      <c r="F73" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="G73" s="31" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="74" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A74" s="26"/>
       <c r="B74" s="27"/>
       <c r="C74" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="D74" s="29"/>
+      <c r="E74" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="D74" s="29"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="28" t="s">
+      <c r="F74" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="G74" s="31" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="75" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A75" s="26"/>
       <c r="B75" s="27"/>
       <c r="C75" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="D75" s="29"/>
-      <c r="E75" s="30"/>
-      <c r="F75" s="29"/>
-      <c r="G75" s="31" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="76" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A76" s="26"/>
       <c r="B76" s="27"/>
       <c r="C76" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="D76" s="29"/>
+      <c r="E76" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="D76" s="29"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="28" t="s">
+      <c r="F76" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="G76" s="31" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="77" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A77" s="26"/>
       <c r="B77" s="27"/>
       <c r="C77" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D77" s="29"/>
-      <c r="E77" s="30"/>
-      <c r="F77" s="29"/>
-      <c r="G77" s="31" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" s="24" customFormat="1" ht="75">
+      <c r="E77" s="29"/>
+      <c r="F77" s="31" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" s="24" customFormat="1" ht="75">
       <c r="A78" s="26"/>
       <c r="B78" s="27"/>
       <c r="C78" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="D78" s="29"/>
+      <c r="E78" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="D78" s="29"/>
-      <c r="E78" s="30"/>
-      <c r="F78" s="28" t="s">
+      <c r="F78" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="G78" s="31" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="79" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A79" s="26"/>
       <c r="B79" s="27"/>
       <c r="C79" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="D79" s="29"/>
+      <c r="E79" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="D79" s="29"/>
-      <c r="E79" s="30"/>
-      <c r="F79" s="28" t="s">
+      <c r="F79" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="G79" s="31" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="80" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A80" s="26"/>
       <c r="B80" s="27"/>
       <c r="C80" s="28" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D80" s="29"/>
-      <c r="E80" s="30"/>
-      <c r="F80" s="29"/>
-      <c r="G80" s="30"/>
-    </row>
-    <row r="81" spans="1:7" s="24" customFormat="1">
+      <c r="E80" s="29"/>
+      <c r="F80" s="30"/>
+    </row>
+    <row r="81" spans="1:6" s="24" customFormat="1">
       <c r="A81" s="26"/>
       <c r="B81" s="27"/>
       <c r="C81" s="28"/>
       <c r="D81" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="E81" s="29"/>
+      <c r="F81" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="E81" s="30"/>
-      <c r="F81" s="29"/>
-      <c r="G81" s="31" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="82" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A82" s="26"/>
       <c r="B82" s="27"/>
       <c r="C82" s="28"/>
       <c r="D82" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="E82" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="E82" s="30"/>
-      <c r="F82" s="28" t="s">
+      <c r="F82" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="G82" s="31" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="83" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A83" s="26"/>
       <c r="B83" s="27"/>
       <c r="C83" s="28"/>
       <c r="D83" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="E83" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="E83" s="30"/>
-      <c r="F83" s="28" t="s">
+      <c r="F83" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="G83" s="31" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="84" spans="1:6" s="24" customFormat="1">
       <c r="A84" s="26"/>
       <c r="B84" s="27"/>
       <c r="C84" s="28"/>
       <c r="D84" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="E84" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="E84" s="30"/>
-      <c r="F84" s="29" t="s">
+      <c r="F84" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="G84" s="31" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="85" spans="1:6" s="24" customFormat="1">
       <c r="A85" s="26"/>
       <c r="B85" s="27"/>
       <c r="C85" s="28"/>
       <c r="D85" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="E85" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="F85" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="E85" s="30"/>
-      <c r="F85" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="G85" s="31" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="86" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A86" s="26"/>
       <c r="B86" s="27"/>
       <c r="C86" s="28"/>
       <c r="D86" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="E86" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="E86" s="30"/>
-      <c r="F86" s="28" t="s">
+      <c r="F86" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="G86" s="31" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="87" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A87" s="26"/>
       <c r="B87" s="27"/>
       <c r="C87" s="28"/>
       <c r="D87" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="E87" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="E87" s="30"/>
-      <c r="F87" s="28" t="s">
+      <c r="F87" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="G87" s="31" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="88" spans="1:6" s="24" customFormat="1">
       <c r="A88" s="26"/>
       <c r="B88" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C88" s="29"/>
       <c r="D88" s="29"/>
-      <c r="E88" s="30"/>
-      <c r="F88" s="29"/>
-      <c r="G88" s="30"/>
-    </row>
-    <row r="89" spans="1:7" s="24" customFormat="1" ht="45">
+      <c r="E88" s="29"/>
+      <c r="F88" s="30"/>
+    </row>
+    <row r="89" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A89" s="26"/>
       <c r="B89" s="32"/>
       <c r="C89" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="D89" s="29"/>
+      <c r="E89" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="D89" s="29"/>
-      <c r="E89" s="30"/>
-      <c r="F89" s="28" t="s">
+      <c r="F89" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="G89" s="31" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="90" spans="1:6" s="24" customFormat="1">
       <c r="A90" s="26"/>
       <c r="B90" s="32"/>
       <c r="C90" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="D90" s="29"/>
-      <c r="E90" s="30"/>
-      <c r="F90" s="29" t="s">
+      <c r="F90" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="G90" s="31" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" s="24" customFormat="1" ht="120">
+    </row>
+    <row r="91" spans="1:6" s="24" customFormat="1" ht="90">
       <c r="A91" s="26"/>
       <c r="B91" s="32"/>
       <c r="C91" s="29" t="s">
+        <v>226</v>
+      </c>
+      <c r="D91" s="29"/>
+      <c r="E91" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="D91" s="29"/>
-      <c r="E91" s="30"/>
-      <c r="F91" s="28" t="s">
+      <c r="F91" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="G91" s="31" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="92" spans="1:6" s="24" customFormat="1">
       <c r="A92" s="26"/>
       <c r="B92" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C92" s="29"/>
       <c r="D92" s="29"/>
-      <c r="E92" s="30"/>
-      <c r="F92" s="29"/>
-      <c r="G92" s="30"/>
-    </row>
-    <row r="93" spans="1:7" s="24" customFormat="1" ht="60">
+      <c r="E92" s="29"/>
+      <c r="F92" s="30"/>
+    </row>
+    <row r="93" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A93" s="26"/>
       <c r="B93" s="32"/>
       <c r="C93" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="D93" s="29"/>
+      <c r="E93" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="D93" s="29"/>
-      <c r="E93" s="30"/>
-      <c r="F93" s="28" t="s">
+      <c r="F93" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="G93" s="31" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="94" spans="1:6" s="24" customFormat="1">
       <c r="A94" s="26"/>
       <c r="B94" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C94" s="29"/>
       <c r="D94" s="29"/>
-      <c r="E94" s="30"/>
-      <c r="F94" s="29"/>
-      <c r="G94" s="30"/>
-    </row>
-    <row r="95" spans="1:7" s="24" customFormat="1" ht="30">
+      <c r="E94" s="29"/>
+      <c r="F94" s="30"/>
+    </row>
+    <row r="95" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A95" s="26"/>
       <c r="B95" s="32"/>
       <c r="C95" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="D95" s="29"/>
+      <c r="E95" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="D95" s="29"/>
-      <c r="E95" s="30"/>
-      <c r="F95" s="28" t="s">
+      <c r="F95" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="G95" s="31" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="96" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A96" s="26"/>
       <c r="B96" s="32"/>
       <c r="C96" s="29" t="s">
+        <v>236</v>
+      </c>
+      <c r="D96" s="29"/>
+      <c r="E96" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="F96" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="D96" s="29"/>
-      <c r="E96" s="30"/>
-      <c r="F96" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="G96" s="31" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="97" spans="1:6" s="24" customFormat="1">
       <c r="A97" s="26"/>
       <c r="B97" s="32"/>
       <c r="C97" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="D97" s="29"/>
-      <c r="E97" s="30"/>
-      <c r="F97" s="29" t="s">
+      <c r="F97" s="31" t="s">
         <v>240</v>
       </c>
-      <c r="G97" s="31" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" s="24" customFormat="1" ht="150">
+    </row>
+    <row r="98" spans="1:6" s="24" customFormat="1" ht="135">
       <c r="A98" s="26"/>
       <c r="B98" s="32"/>
       <c r="C98" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="D98" s="29"/>
+      <c r="E98" s="28" t="s">
         <v>242</v>
       </c>
-      <c r="D98" s="29"/>
-      <c r="E98" s="30"/>
-      <c r="F98" s="28" t="s">
+      <c r="F98" s="31" t="s">
         <v>243</v>
       </c>
-      <c r="G98" s="31" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="99" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A99" s="26"/>
       <c r="B99" s="32"/>
       <c r="C99" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="D99" s="29"/>
+      <c r="E99" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="F99" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="D99" s="29"/>
-      <c r="E99" s="30"/>
-      <c r="F99" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="G99" s="31" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" s="24" customFormat="1" ht="120">
+    </row>
+    <row r="100" spans="1:6" s="24" customFormat="1" ht="75">
       <c r="A100" s="26"/>
       <c r="B100" s="32"/>
       <c r="C100" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="D100" s="29"/>
+      <c r="E100" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="D100" s="29"/>
-      <c r="E100" s="30"/>
-      <c r="F100" s="28" t="s">
+      <c r="F100" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="G100" s="31" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="101" spans="1:6" s="24" customFormat="1">
       <c r="A101" s="26"/>
       <c r="B101" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C101" s="29"/>
       <c r="D101" s="29"/>
-      <c r="E101" s="30"/>
-      <c r="F101" s="29"/>
-      <c r="G101" s="30"/>
-    </row>
-    <row r="102" spans="1:7" s="24" customFormat="1" ht="75">
+      <c r="E101" s="29"/>
+      <c r="F101" s="30"/>
+    </row>
+    <row r="102" spans="1:6" s="24" customFormat="1" ht="75">
       <c r="A102" s="26"/>
       <c r="B102" s="32"/>
       <c r="C102" s="29" t="s">
+        <v>250</v>
+      </c>
+      <c r="D102" s="29"/>
+      <c r="E102" s="28" t="s">
         <v>251</v>
       </c>
-      <c r="D102" s="29"/>
-      <c r="E102" s="30"/>
-      <c r="F102" s="28" t="s">
+      <c r="F102" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="G102" s="31" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="103" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A103" s="26"/>
       <c r="B103" s="32"/>
       <c r="C103" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="D103" s="29"/>
+      <c r="E103" s="28" t="s">
         <v>254</v>
       </c>
-      <c r="D103" s="29"/>
-      <c r="E103" s="30"/>
-      <c r="F103" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="G103" s="33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="24" customFormat="1">
+      <c r="F103" s="33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" s="24" customFormat="1">
       <c r="A104" s="26"/>
       <c r="B104" s="32"/>
       <c r="C104" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="D104" s="29"/>
+      <c r="E104" s="29" t="s">
         <v>256</v>
       </c>
-      <c r="D104" s="29"/>
-      <c r="E104" s="30"/>
-      <c r="F104" s="29" t="s">
+      <c r="F104" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="G104" s="31" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="105" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A105" s="26"/>
       <c r="B105" s="32"/>
       <c r="C105" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="D105" s="29"/>
+      <c r="E105" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="D105" s="29"/>
-      <c r="E105" s="30"/>
-      <c r="F105" s="28" t="s">
+      <c r="F105" s="31" t="s">
         <v>260</v>
       </c>
-      <c r="G105" s="31" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="106" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A106" s="26"/>
       <c r="B106" s="32"/>
       <c r="C106" s="29" t="s">
+        <v>261</v>
+      </c>
+      <c r="D106" s="29"/>
+      <c r="E106" s="28" t="s">
         <v>262</v>
       </c>
-      <c r="D106" s="29"/>
-      <c r="E106" s="30"/>
-      <c r="F106" s="28" t="s">
+      <c r="F106" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="G106" s="31" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="107" spans="1:6" s="24" customFormat="1">
       <c r="A107" s="26"/>
       <c r="B107" s="32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C107" s="29"/>
       <c r="D107" s="29"/>
-      <c r="E107" s="30"/>
-      <c r="F107" s="29"/>
-      <c r="G107" s="30"/>
-    </row>
-    <row r="108" spans="1:7" s="24" customFormat="1" ht="30">
+      <c r="E107" s="29"/>
+      <c r="F107" s="30"/>
+    </row>
+    <row r="108" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A108" s="26"/>
       <c r="B108" s="32"/>
       <c r="C108" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="D108" s="29"/>
+      <c r="E108" s="28" t="s">
         <v>266</v>
       </c>
-      <c r="D108" s="29"/>
-      <c r="E108" s="30"/>
-      <c r="F108" s="28" t="s">
+      <c r="F108" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="G108" s="31" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="109" spans="1:6" s="24" customFormat="1">
       <c r="A109" s="26"/>
       <c r="B109" s="32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C109" s="29"/>
       <c r="D109" s="29"/>
-      <c r="E109" s="30"/>
-      <c r="F109" s="29"/>
-      <c r="G109" s="30"/>
-    </row>
-    <row r="110" spans="1:7" s="24" customFormat="1" ht="30">
+      <c r="E109" s="29"/>
+      <c r="F109" s="30"/>
+    </row>
+    <row r="110" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A110" s="26"/>
       <c r="B110" s="32"/>
       <c r="C110" s="29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D110" s="29"/>
-      <c r="E110" s="30"/>
-      <c r="F110" s="28" t="s">
+      <c r="E110" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="F110" s="31" t="s">
         <v>270</v>
       </c>
-      <c r="G110" s="31" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="111" spans="1:6" s="24" customFormat="1">
       <c r="A111" s="26"/>
       <c r="B111" s="32"/>
       <c r="C111" s="29" t="s">
+        <v>271</v>
+      </c>
+      <c r="D111" s="29"/>
+      <c r="E111" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="D111" s="29"/>
-      <c r="E111" s="30"/>
-      <c r="F111" s="29" t="s">
+      <c r="F111" s="31" t="s">
         <v>273</v>
       </c>
-      <c r="G111" s="31" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="112" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A112" s="26"/>
       <c r="B112" s="32"/>
       <c r="C112" s="29" t="s">
+        <v>274</v>
+      </c>
+      <c r="D112" s="29"/>
+      <c r="E112" s="28" t="s">
         <v>275</v>
       </c>
-      <c r="D112" s="29"/>
-      <c r="E112" s="30"/>
-      <c r="F112" s="28" t="s">
+      <c r="F112" s="31" t="s">
         <v>276</v>
       </c>
-      <c r="G112" s="31" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="113" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A113" s="26"/>
       <c r="B113" s="32"/>
       <c r="C113" s="29" t="s">
+        <v>277</v>
+      </c>
+      <c r="D113" s="29"/>
+      <c r="E113" s="28" t="s">
         <v>278</v>
       </c>
-      <c r="D113" s="29"/>
-      <c r="E113" s="30"/>
-      <c r="F113" s="28" t="s">
+      <c r="F113" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="G113" s="31" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" s="24" customFormat="1" ht="135">
+    </row>
+    <row r="114" spans="1:6" s="24" customFormat="1" ht="75">
       <c r="A114" s="26"/>
       <c r="B114" s="32"/>
       <c r="C114" s="29" t="s">
+        <v>280</v>
+      </c>
+      <c r="D114" s="29"/>
+      <c r="E114" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="D114" s="29"/>
-      <c r="E114" s="30"/>
-      <c r="F114" s="28" t="s">
+      <c r="F114" s="31" t="s">
         <v>282</v>
       </c>
-      <c r="G114" s="31" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" s="24" customFormat="1" ht="105">
+    </row>
+    <row r="115" spans="1:6" s="24" customFormat="1" ht="105">
       <c r="A115" s="26"/>
       <c r="B115" s="32"/>
       <c r="C115" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="D115" s="29"/>
+      <c r="E115" s="28" t="s">
         <v>284</v>
       </c>
-      <c r="D115" s="29"/>
-      <c r="E115" s="30"/>
-      <c r="F115" s="28" t="s">
+      <c r="F115" s="31" t="s">
         <v>285</v>
       </c>
-      <c r="G115" s="31" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="116" spans="1:6" s="24" customFormat="1">
       <c r="A116" s="26"/>
       <c r="B116" s="32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C116" s="29"/>
       <c r="D116" s="29"/>
-      <c r="E116" s="30"/>
-      <c r="F116" s="29"/>
-      <c r="G116" s="30"/>
-    </row>
-    <row r="117" spans="1:7" s="24" customFormat="1" ht="60">
+      <c r="E116" s="29"/>
+      <c r="F116" s="30"/>
+    </row>
+    <row r="117" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A117" s="26"/>
       <c r="B117" s="32"/>
       <c r="C117" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="D117" s="29"/>
+      <c r="E117" s="28" t="s">
         <v>287</v>
       </c>
-      <c r="D117" s="29"/>
-      <c r="E117" s="30"/>
-      <c r="F117" s="28" t="s">
+      <c r="F117" s="31" t="s">
         <v>288</v>
       </c>
-      <c r="G117" s="31" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="118" spans="1:6" s="24" customFormat="1">
       <c r="A118" s="26"/>
       <c r="B118" s="32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C118" s="29"/>
       <c r="D118" s="29"/>
-      <c r="E118" s="30"/>
-      <c r="F118" s="29"/>
-      <c r="G118" s="30"/>
-    </row>
-    <row r="119" spans="1:7" s="24" customFormat="1">
+      <c r="E118" s="29"/>
+      <c r="F118" s="30"/>
+    </row>
+    <row r="119" spans="1:6" s="24" customFormat="1">
       <c r="A119" s="26"/>
       <c r="B119" s="32"/>
       <c r="C119" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="D119" s="29"/>
+      <c r="E119" s="29" t="s">
         <v>291</v>
       </c>
-      <c r="D119" s="29"/>
-      <c r="E119" s="30"/>
-      <c r="F119" s="29" t="s">
+      <c r="F119" s="31" t="s">
         <v>292</v>
       </c>
-      <c r="G119" s="31" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="120" spans="1:6" s="24" customFormat="1">
       <c r="A120" s="26"/>
       <c r="B120" s="32"/>
       <c r="C120" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="D120" s="29"/>
+      <c r="E120" s="29" t="s">
         <v>294</v>
       </c>
-      <c r="D120" s="29"/>
-      <c r="E120" s="30"/>
-      <c r="F120" s="29" t="s">
+      <c r="F120" s="31" t="s">
         <v>295</v>
       </c>
-      <c r="G120" s="31" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="121" spans="1:6" s="24" customFormat="1">
       <c r="A121" s="26"/>
       <c r="B121" s="32"/>
       <c r="C121" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="D121" s="29"/>
+      <c r="E121" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="F121" s="31" t="s">
         <v>297</v>
       </c>
-      <c r="D121" s="29"/>
-      <c r="E121" s="30"/>
-      <c r="F121" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="G121" s="31" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="122" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A122" s="26"/>
       <c r="B122" s="32"/>
       <c r="C122" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="D122" s="29"/>
+      <c r="E122" s="28" t="s">
         <v>299</v>
       </c>
-      <c r="D122" s="29"/>
-      <c r="E122" s="30"/>
-      <c r="F122" s="28" t="s">
+      <c r="F122" s="33" t="s">
         <v>300</v>
       </c>
-      <c r="G122" s="33" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" s="24" customFormat="1" ht="120">
+    </row>
+    <row r="123" spans="1:6" s="24" customFormat="1" ht="90">
       <c r="A123" s="26"/>
       <c r="B123" s="27"/>
       <c r="C123" s="28" t="s">
+        <v>301</v>
+      </c>
+      <c r="D123" s="29"/>
+      <c r="E123" s="28" t="s">
         <v>302</v>
       </c>
-      <c r="D123" s="29"/>
-      <c r="E123" s="30"/>
-      <c r="F123" s="28" t="s">
+      <c r="F123" s="31" t="s">
         <v>303</v>
       </c>
-      <c r="G123" s="31" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="124" spans="1:6" s="24" customFormat="1">
       <c r="A124" s="26"/>
       <c r="B124" s="27"/>
       <c r="C124" s="28" t="s">
+        <v>304</v>
+      </c>
+      <c r="D124" s="29"/>
+      <c r="E124" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="D124" s="29"/>
-      <c r="E124" s="30"/>
-      <c r="F124" s="29" t="s">
+      <c r="F124" s="31" t="s">
         <v>306</v>
       </c>
-      <c r="G124" s="31" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="125" spans="1:6" s="24" customFormat="1">
       <c r="A125" s="26"/>
       <c r="B125" s="27"/>
       <c r="C125" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="D125" s="29"/>
+      <c r="E125" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="F125" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="D125" s="29"/>
-      <c r="E125" s="30"/>
-      <c r="F125" s="29" t="s">
-        <v>240</v>
-      </c>
-      <c r="G125" s="31" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="126" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A126" s="26"/>
       <c r="B126" s="27"/>
       <c r="C126" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="D126" s="29"/>
+      <c r="E126" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="D126" s="29"/>
-      <c r="E126" s="30"/>
-      <c r="F126" s="28" t="s">
+      <c r="F126" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="G126" s="31" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="127" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A127" s="26"/>
       <c r="B127" s="27"/>
       <c r="C127" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="D127" s="29"/>
+      <c r="E127" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="D127" s="29"/>
-      <c r="E127" s="30"/>
-      <c r="F127" s="28" t="s">
+      <c r="F127" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="G127" s="31" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="128" spans="1:6" s="24" customFormat="1">
       <c r="A128" s="26"/>
       <c r="B128" s="27"/>
       <c r="C128" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="D128" s="29"/>
+      <c r="E128" s="29"/>
+      <c r="F128" s="31" t="s">
         <v>316</v>
       </c>
-      <c r="D128" s="29"/>
-      <c r="E128" s="30"/>
-      <c r="F128" s="29"/>
-      <c r="G128" s="31" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="129" spans="1:6" s="24" customFormat="1">
       <c r="A129" s="26"/>
       <c r="B129" s="27" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C129" s="28"/>
       <c r="D129" s="29"/>
-      <c r="E129" s="30"/>
-      <c r="F129" s="29"/>
-      <c r="G129" s="30"/>
-    </row>
-    <row r="130" spans="1:7" s="24" customFormat="1">
+      <c r="E129" s="29"/>
+      <c r="F129" s="30"/>
+    </row>
+    <row r="130" spans="1:6" s="24" customFormat="1">
       <c r="A130" s="26"/>
       <c r="B130" s="27"/>
       <c r="C130" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="D130" s="29"/>
+      <c r="E130" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="D130" s="29"/>
-      <c r="E130" s="30"/>
-      <c r="F130" s="29" t="s">
+      <c r="F130" s="31" t="s">
         <v>320</v>
       </c>
-      <c r="G130" s="31" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" s="24" customFormat="1" ht="195">
+    </row>
+    <row r="131" spans="1:6" s="24" customFormat="1" ht="135">
       <c r="A131" s="26"/>
       <c r="B131" s="27"/>
       <c r="C131" s="28" t="s">
+        <v>321</v>
+      </c>
+      <c r="D131" s="29"/>
+      <c r="E131" s="28" t="s">
         <v>322</v>
       </c>
-      <c r="D131" s="29"/>
-      <c r="E131" s="30"/>
-      <c r="F131" s="28" t="s">
+      <c r="F131" s="31" t="s">
         <v>323</v>
       </c>
-      <c r="G131" s="31" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" s="24" customFormat="1" ht="240">
+    </row>
+    <row r="132" spans="1:6" s="24" customFormat="1" ht="180">
       <c r="A132" s="26"/>
       <c r="B132" s="27"/>
       <c r="C132" s="28" t="s">
+        <v>324</v>
+      </c>
+      <c r="D132" s="29"/>
+      <c r="E132" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="D132" s="29"/>
-      <c r="E132" s="30"/>
-      <c r="F132" s="28" t="s">
+      <c r="F132" s="31" t="s">
         <v>326</v>
       </c>
-      <c r="G132" s="31" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" s="24" customFormat="1" ht="150">
+    </row>
+    <row r="133" spans="1:6" s="24" customFormat="1" ht="150">
       <c r="A133" s="26"/>
       <c r="B133" s="27"/>
       <c r="C133" s="28" t="s">
+        <v>327</v>
+      </c>
+      <c r="D133" s="29"/>
+      <c r="E133" s="28" t="s">
         <v>328</v>
       </c>
-      <c r="D133" s="29"/>
-      <c r="E133" s="30"/>
-      <c r="F133" s="28" t="s">
+      <c r="F133" s="31" t="s">
         <v>329</v>
       </c>
-      <c r="G133" s="31" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="134" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A134" s="26"/>
       <c r="B134" s="27"/>
       <c r="C134" s="28" t="s">
+        <v>330</v>
+      </c>
+      <c r="D134" s="29"/>
+      <c r="E134" s="28" t="s">
         <v>331</v>
       </c>
-      <c r="D134" s="29"/>
-      <c r="E134" s="30"/>
-      <c r="F134" s="28" t="s">
+      <c r="F134" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="G134" s="31" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="135" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A135" s="26"/>
       <c r="B135" s="27"/>
       <c r="C135" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="D135" s="29"/>
+      <c r="E135" s="28" t="s">
         <v>334</v>
       </c>
-      <c r="D135" s="29"/>
-      <c r="E135" s="30"/>
-      <c r="F135" s="28" t="s">
+      <c r="F135" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="G135" s="31" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="136" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A136" s="26"/>
       <c r="B136" s="27"/>
       <c r="C136" s="28" t="s">
+        <v>336</v>
+      </c>
+      <c r="D136" s="29"/>
+      <c r="E136" s="28" t="s">
         <v>337</v>
       </c>
-      <c r="D136" s="29"/>
-      <c r="E136" s="30"/>
-      <c r="F136" s="28" t="s">
+      <c r="F136" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="G136" s="31" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="137" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A137" s="26"/>
       <c r="B137" s="27"/>
       <c r="C137" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="D137" s="29"/>
+      <c r="E137" s="28" t="s">
         <v>340</v>
       </c>
-      <c r="D137" s="29"/>
-      <c r="E137" s="30"/>
-      <c r="F137" s="28" t="s">
+      <c r="F137" s="31" t="s">
         <v>341</v>
       </c>
-      <c r="G137" s="31" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="138" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A138" s="26"/>
       <c r="B138" s="27"/>
       <c r="C138" s="28" t="s">
+        <v>342</v>
+      </c>
+      <c r="D138" s="29"/>
+      <c r="E138" s="28" t="s">
         <v>343</v>
       </c>
-      <c r="D138" s="29"/>
-      <c r="E138" s="30"/>
-      <c r="F138" s="28" t="s">
+      <c r="F138" s="31" t="s">
         <v>344</v>
       </c>
-      <c r="G138" s="31" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="139" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A139" s="26"/>
       <c r="B139" s="27"/>
       <c r="C139" s="28" t="s">
+        <v>345</v>
+      </c>
+      <c r="D139" s="29"/>
+      <c r="E139" s="28" t="s">
         <v>346</v>
       </c>
-      <c r="D139" s="29"/>
-      <c r="E139" s="30"/>
-      <c r="F139" s="28" t="s">
+      <c r="F139" s="31" t="s">
         <v>347</v>
       </c>
-      <c r="G139" s="31" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="140" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A140" s="26"/>
       <c r="B140" s="27"/>
       <c r="C140" s="28" t="s">
+        <v>348</v>
+      </c>
+      <c r="D140" s="29"/>
+      <c r="E140" s="28" t="s">
         <v>349</v>
       </c>
-      <c r="D140" s="29"/>
-      <c r="E140" s="30"/>
-      <c r="F140" s="28" t="s">
+      <c r="F140" s="31" t="s">
         <v>350</v>
       </c>
-      <c r="G140" s="31" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" s="24" customFormat="1" ht="75">
+    </row>
+    <row r="141" spans="1:6" s="24" customFormat="1" ht="75">
       <c r="A141" s="26"/>
       <c r="B141" s="27"/>
       <c r="C141" s="28" t="s">
+        <v>351</v>
+      </c>
+      <c r="D141" s="29"/>
+      <c r="E141" s="28" t="s">
         <v>352</v>
       </c>
-      <c r="D141" s="29"/>
-      <c r="E141" s="30"/>
-      <c r="F141" s="28" t="s">
+      <c r="F141" s="31" t="s">
         <v>353</v>
       </c>
-      <c r="G141" s="31" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" s="24" customFormat="1" ht="105">
+    </row>
+    <row r="142" spans="1:6" s="24" customFormat="1" ht="90">
       <c r="A142" s="26"/>
       <c r="B142" s="27"/>
       <c r="C142" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="D142" s="29"/>
+      <c r="E142" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="D142" s="29"/>
-      <c r="E142" s="30"/>
-      <c r="F142" s="28" t="s">
+      <c r="F142" s="31" t="s">
         <v>356</v>
       </c>
-      <c r="G142" s="31" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="143" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A143" s="26"/>
       <c r="B143" s="27"/>
       <c r="C143" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="D143" s="29"/>
+      <c r="E143" s="28" t="s">
         <v>358</v>
       </c>
-      <c r="D143" s="29"/>
-      <c r="E143" s="30"/>
-      <c r="F143" s="28" t="s">
+      <c r="F143" s="31" t="s">
         <v>359</v>
       </c>
-      <c r="G143" s="31" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="144" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A144" s="26"/>
       <c r="B144" s="27"/>
       <c r="C144" s="28" t="s">
+        <v>360</v>
+      </c>
+      <c r="D144" s="29"/>
+      <c r="E144" s="28" t="s">
         <v>361</v>
       </c>
-      <c r="D144" s="29"/>
-      <c r="E144" s="30"/>
-      <c r="F144" s="28" t="s">
+      <c r="F144" s="31" t="s">
         <v>362</v>
       </c>
-      <c r="G144" s="31" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" s="24" customFormat="1" ht="120">
+    </row>
+    <row r="145" spans="1:6" s="24" customFormat="1" ht="75">
       <c r="A145" s="26"/>
       <c r="B145" s="27"/>
       <c r="C145" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="D145" s="29"/>
+      <c r="E145" s="28" t="s">
         <v>364</v>
       </c>
-      <c r="D145" s="29"/>
-      <c r="E145" s="30"/>
-      <c r="F145" s="28" t="s">
+      <c r="F145" s="31" t="s">
         <v>365</v>
       </c>
-      <c r="G145" s="31" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="146" spans="1:6" s="24" customFormat="1" ht="60">
       <c r="A146" s="26"/>
       <c r="B146" s="27"/>
       <c r="C146" s="28" t="s">
+        <v>366</v>
+      </c>
+      <c r="D146" s="29"/>
+      <c r="E146" s="28" t="s">
         <v>367</v>
       </c>
-      <c r="D146" s="29"/>
-      <c r="E146" s="30"/>
-      <c r="F146" s="28" t="s">
+      <c r="F146" s="31" t="s">
         <v>368</v>
       </c>
-      <c r="G146" s="31" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" s="24" customFormat="1" ht="75">
+    </row>
+    <row r="147" spans="1:6" s="24" customFormat="1" ht="75">
       <c r="A147" s="26"/>
       <c r="B147" s="27"/>
       <c r="C147" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="D147" s="29"/>
+      <c r="E147" s="28" t="s">
         <v>370</v>
       </c>
-      <c r="D147" s="29"/>
-      <c r="E147" s="30"/>
-      <c r="F147" s="28" t="s">
+      <c r="F147" s="31" t="s">
         <v>371</v>
       </c>
-      <c r="G147" s="31" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" s="24" customFormat="1" ht="60">
+    </row>
+    <row r="148" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A148" s="26"/>
       <c r="B148" s="27"/>
       <c r="C148" s="28" t="s">
+        <v>372</v>
+      </c>
+      <c r="D148" s="29"/>
+      <c r="E148" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="D148" s="29"/>
-      <c r="E148" s="30"/>
-      <c r="F148" s="28" t="s">
+      <c r="F148" s="31" t="s">
         <v>374</v>
       </c>
-      <c r="G148" s="31" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="149" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A149" s="26"/>
       <c r="B149" s="27"/>
       <c r="C149" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="D149" s="29"/>
+      <c r="E149" s="28" t="s">
         <v>376</v>
       </c>
-      <c r="D149" s="29"/>
-      <c r="E149" s="30"/>
-      <c r="F149" s="28" t="s">
+      <c r="F149" s="31" t="s">
         <v>377</v>
       </c>
-      <c r="G149" s="31" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="150" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A150" s="26"/>
       <c r="B150" s="27"/>
       <c r="C150" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="D150" s="29"/>
+      <c r="E150" s="28" t="s">
         <v>379</v>
       </c>
-      <c r="D150" s="29"/>
-      <c r="E150" s="30"/>
-      <c r="F150" s="28" t="s">
+      <c r="F150" s="31" t="s">
         <v>380</v>
       </c>
-      <c r="G150" s="31" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" s="24" customFormat="1" ht="30">
+    </row>
+    <row r="151" spans="1:6" s="24" customFormat="1" ht="30">
       <c r="A151" s="26"/>
       <c r="B151" s="27"/>
       <c r="C151" s="28" t="s">
+        <v>381</v>
+      </c>
+      <c r="D151" s="29"/>
+      <c r="E151" s="28" t="s">
         <v>382</v>
       </c>
-      <c r="D151" s="29"/>
-      <c r="E151" s="30"/>
-      <c r="F151" s="28" t="s">
+      <c r="F151" s="31" t="s">
         <v>383</v>
       </c>
-      <c r="G151" s="31" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="152" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A152" s="26"/>
       <c r="B152" s="27"/>
       <c r="C152" s="28" t="s">
+        <v>384</v>
+      </c>
+      <c r="D152" s="29"/>
+      <c r="E152" s="28" t="s">
         <v>385</v>
       </c>
-      <c r="D152" s="29"/>
-      <c r="E152" s="30"/>
-      <c r="F152" s="28" t="s">
+      <c r="F152" s="31" t="s">
         <v>386</v>
       </c>
-      <c r="G152" s="31" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" s="24" customFormat="1">
+    </row>
+    <row r="153" spans="1:6" s="24" customFormat="1">
       <c r="A153" s="26"/>
       <c r="B153" s="27"/>
       <c r="C153" s="28" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D153" s="29"/>
-      <c r="E153" s="30"/>
-      <c r="F153" s="29"/>
-      <c r="G153" s="30"/>
-    </row>
-    <row r="154" spans="1:7" s="24" customFormat="1" ht="75">
+      <c r="E153" s="29"/>
+      <c r="F153" s="30"/>
+    </row>
+    <row r="154" spans="1:6" s="24" customFormat="1" ht="75">
       <c r="A154" s="26"/>
       <c r="B154" s="27"/>
       <c r="C154" s="28"/>
       <c r="D154" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="E154" s="28" t="s">
         <v>389</v>
       </c>
-      <c r="E154" s="30"/>
-      <c r="F154" s="28" t="s">
+      <c r="F154" s="31" t="s">
         <v>390</v>
       </c>
-      <c r="G154" s="31" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" s="24" customFormat="1" ht="45">
+    </row>
+    <row r="155" spans="1:6" s="24" customFormat="1" ht="45">
       <c r="A155" s="26"/>
       <c r="B155" s="27"/>
       <c r="C155" s="28"/>
       <c r="D155" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="E155" s="28" t="s">
         <v>392</v>
       </c>
-      <c r="E155" s="30"/>
-      <c r="F155" s="28" t="s">
+      <c r="F155" s="31" t="s">
         <v>393</v>
-      </c>
-      <c r="G155" s="31" t="s">
-        <v>394</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{93A3DA59-A425-42B4-8D5F-58614DBB0F5B}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{6A4E133A-7492-4221-B4CB-1EF3B0AB94D0}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{FFD8CADC-5728-4ABB-9956-70A6F447CC2C}"/>
-    <hyperlink ref="G6" r:id="rId4" xr:uid="{D013559B-C157-4E85-9A8C-C6E7B9881BDB}"/>
-    <hyperlink ref="G8" r:id="rId5" xr:uid="{5730BF1F-46E4-4897-879A-176A89C130A5}"/>
-    <hyperlink ref="G9" r:id="rId6" xr:uid="{4D8B7151-1212-4EBD-A397-486C81979B4C}"/>
-    <hyperlink ref="G10" r:id="rId7" xr:uid="{86F66F59-F1D3-4071-BBF0-8010B161B8E5}"/>
-    <hyperlink ref="G11" r:id="rId8" xr:uid="{2D8970E9-447B-42C2-A88D-A2C765B8617D}"/>
-    <hyperlink ref="G13" r:id="rId9" location="building-and-deploying-mrtk-to-hololens-1-and-hololens-2-uwp" xr:uid="{71AF9FF5-8B79-4A5E-94D2-2B30B05E611E}"/>
-    <hyperlink ref="G14" r:id="rId10" xr:uid="{B64CEDE7-5C9A-446A-9344-9AA23CAAF32C}"/>
-    <hyperlink ref="G15" r:id="rId11" xr:uid="{8DC6C39F-E9AB-4D54-A755-88A3F4F9CC2E}"/>
-    <hyperlink ref="G16" r:id="rId12" location="finding-the-current-version" xr:uid="{2E9E623A-32DE-464C-9016-6358575FBC7E}"/>
-    <hyperlink ref="G18" r:id="rId13" xr:uid="{D6EB05E2-FF4D-4F2E-8CCF-761BF38C3456}"/>
-    <hyperlink ref="G19" r:id="rId14" xr:uid="{F38F93B5-24D2-4784-8B82-6E1EBBA7881C}"/>
-    <hyperlink ref="G21" r:id="rId15" xr:uid="{ADF6E112-9990-4660-B1A8-FF7BF284742A}"/>
-    <hyperlink ref="G22" r:id="rId16" xr:uid="{49EBDDB4-2E4C-4855-9AE0-FDBD4D801881}"/>
-    <hyperlink ref="G23" r:id="rId17" xr:uid="{11CE312F-0283-4B88-B42B-B489A3793E64}"/>
-    <hyperlink ref="G25" r:id="rId18" xr:uid="{5E5CC973-FB34-4E0D-8465-A736DD70BD69}"/>
-    <hyperlink ref="G26" r:id="rId19" xr:uid="{89E341CC-6F40-4B2C-90FF-F45082C6597F}"/>
-    <hyperlink ref="G28" r:id="rId20" xr:uid="{3854E21E-81F2-4C0D-894F-58CF18910E54}"/>
-    <hyperlink ref="G29" r:id="rId21" xr:uid="{B277221E-CB8C-4ED3-AAAB-DDEA402EA2D8}"/>
-    <hyperlink ref="G30" r:id="rId22" xr:uid="{981DD41E-1D06-4B57-A808-45913634D62E}"/>
-    <hyperlink ref="G31" r:id="rId23" xr:uid="{B337741F-12AB-4AA5-AE43-46FD1313E145}"/>
-    <hyperlink ref="G34" r:id="rId24" xr:uid="{D17E8A7B-5D5D-46D9-BBD6-884A346BE888}"/>
-    <hyperlink ref="G35" r:id="rId25" xr:uid="{4EA77164-7B03-425B-A93C-B54C08184C14}"/>
-    <hyperlink ref="G37" r:id="rId26" xr:uid="{B10F0F97-4FF1-4131-B36D-516E7CBCCC60}"/>
-    <hyperlink ref="G38" r:id="rId27" xr:uid="{07398E30-E603-49F8-85EA-6C026173A549}"/>
-    <hyperlink ref="G39" r:id="rId28" xr:uid="{C8F4A9E4-39F8-42B0-BE8A-796628212166}"/>
-    <hyperlink ref="G40" r:id="rId29" xr:uid="{680D7AAB-C71C-4E05-A455-59970D35D2EF}"/>
-    <hyperlink ref="G42" r:id="rId30" xr:uid="{510B2B6C-F700-4B42-8222-9824F10312AA}"/>
-    <hyperlink ref="G43" r:id="rId31" xr:uid="{A9AE4DED-6750-451F-B2F1-9878F2064B77}"/>
-    <hyperlink ref="G44" r:id="rId32" xr:uid="{97A3FCDE-117F-467B-82EE-49415B13685C}"/>
-    <hyperlink ref="G45" r:id="rId33" xr:uid="{54B09E6C-82C8-4B1B-A90B-EA2189EA7DC1}"/>
-    <hyperlink ref="G47" r:id="rId34" xr:uid="{3F685F22-DEF1-4908-8F14-957B4596873C}"/>
-    <hyperlink ref="G48" r:id="rId35" xr:uid="{8525CEA4-BB37-4962-871B-93BE3F8D8695}"/>
-    <hyperlink ref="G49" r:id="rId36" xr:uid="{99AD427F-01DB-4E95-8AAB-373215FAC669}"/>
-    <hyperlink ref="G51" r:id="rId37" xr:uid="{C41F81C9-8B2A-4BAE-BE13-E0FFE7521B30}"/>
-    <hyperlink ref="G52" r:id="rId38" xr:uid="{7422CF83-A8B3-4972-8898-2E3ECFA7D73B}"/>
-    <hyperlink ref="G53" r:id="rId39" xr:uid="{3281634E-AF79-4C83-8E61-F001F65FBD15}"/>
-    <hyperlink ref="G54" r:id="rId40" xr:uid="{3FF6B46D-5693-483F-9CD2-F6B802552EEB}"/>
-    <hyperlink ref="G56" r:id="rId41" xr:uid="{1FF1D250-458C-41FE-A035-3A1B9E0B6306}"/>
-    <hyperlink ref="G57" r:id="rId42" xr:uid="{4BB4DAA4-48A5-4640-B10F-0CBCD6A3BE12}"/>
-    <hyperlink ref="G58" r:id="rId43" xr:uid="{DB319251-7975-47A0-88CD-66FE8B9D5A62}"/>
-    <hyperlink ref="G59" r:id="rId44" xr:uid="{61A6D1B8-6B13-4B13-8C2C-88D2A085DCB5}"/>
-    <hyperlink ref="G61" r:id="rId45" xr:uid="{A13684DA-A5FB-4215-BF53-D837E5E9C76D}"/>
-    <hyperlink ref="G62" r:id="rId46" xr:uid="{616C1391-EAAB-4EBB-8C50-87D322C11877}"/>
-    <hyperlink ref="G63" r:id="rId47" xr:uid="{449B57F6-DFF2-4AD1-A178-FB6212AF3533}"/>
-    <hyperlink ref="G64" r:id="rId48" xr:uid="{730E491B-25F4-49CA-AD1D-5F5C04A2ADFC}"/>
-    <hyperlink ref="G66" r:id="rId49" xr:uid="{E413D097-57C9-47E5-9B67-6CA9DAC60C2B}"/>
-    <hyperlink ref="G67" r:id="rId50" xr:uid="{B9F69EED-4326-496E-B8AB-9E5072CCD4AC}"/>
-    <hyperlink ref="G68" r:id="rId51" xr:uid="{E8298287-BC71-4C33-8B39-49E93C287430}"/>
-    <hyperlink ref="G69" r:id="rId52" xr:uid="{01C4BCBC-0FAB-4FC0-BB28-ED1413937CC8}"/>
-    <hyperlink ref="G70" r:id="rId53" xr:uid="{4D0370F5-CCC4-4C9D-B5CC-4463BF0B9870}"/>
-    <hyperlink ref="G71" r:id="rId54" xr:uid="{67844097-C438-43EA-B9E0-79595395094B}"/>
-    <hyperlink ref="G72" r:id="rId55" xr:uid="{E3B3DEA8-7B43-4DBD-9942-A48B4BFF60FA}"/>
-    <hyperlink ref="G73" r:id="rId56" xr:uid="{B1446712-A623-43A7-9B4F-69AEB1C02B34}"/>
-    <hyperlink ref="G74" r:id="rId57" xr:uid="{42A7C29B-0D9C-4061-AD34-C34E9E1E5344}"/>
-    <hyperlink ref="G75" r:id="rId58" xr:uid="{3BFB3FB4-DA5C-413D-922F-5358384FBA37}"/>
-    <hyperlink ref="G76" r:id="rId59" xr:uid="{CB67CB8A-E75C-42B9-92A1-B1D711A008A0}"/>
-    <hyperlink ref="G77" r:id="rId60" xr:uid="{BD9A5733-C0BB-4829-95F4-018DD4948471}"/>
-    <hyperlink ref="G78" r:id="rId61" xr:uid="{CB9921CA-A1B1-4C7D-987A-D84886884DE3}"/>
-    <hyperlink ref="G79" r:id="rId62" xr:uid="{325B681B-9A9E-4367-86FD-646A297873A6}"/>
-    <hyperlink ref="G81" r:id="rId63" xr:uid="{7C24BD78-580C-4B83-92CE-4F9A73DF21D1}"/>
-    <hyperlink ref="G82" r:id="rId64" xr:uid="{837FE256-264A-48D1-B4A0-3DC9D41F01D7}"/>
-    <hyperlink ref="G83" r:id="rId65" xr:uid="{0F2B7185-552E-4967-83AC-A300D874A411}"/>
-    <hyperlink ref="G84" r:id="rId66" xr:uid="{3CD22473-AE2E-4B8D-AA0C-DA1A3FD73D3D}"/>
-    <hyperlink ref="G85" r:id="rId67" xr:uid="{464AA96C-2E81-4DD8-971E-FB5A8F22FE54}"/>
-    <hyperlink ref="G86" r:id="rId68" xr:uid="{45CE71C8-7B3B-4152-8E12-920A52C953B8}"/>
-    <hyperlink ref="G87" r:id="rId69" xr:uid="{523C8272-EA14-44CF-9A75-0B5E9776BD07}"/>
-    <hyperlink ref="G89" r:id="rId70" xr:uid="{1A1116FD-CD0C-4E49-88D6-DA7B8E263BC8}"/>
-    <hyperlink ref="G90" r:id="rId71" xr:uid="{81E073F9-AEDE-45AC-A164-27B3119B458B}"/>
-    <hyperlink ref="G91" r:id="rId72" xr:uid="{6F138136-5044-4F83-91EB-B24E0D69A3E0}"/>
-    <hyperlink ref="G93" r:id="rId73" xr:uid="{391F87F3-211E-4A04-B158-DEEBE023F73F}"/>
-    <hyperlink ref="G95" r:id="rId74" xr:uid="{719FAA48-4EC4-4D08-B666-9E72202F5A08}"/>
-    <hyperlink ref="G96" r:id="rId75" xr:uid="{B99681F4-0AC8-4290-B61A-32C580BE0E3E}"/>
-    <hyperlink ref="G97" r:id="rId76" xr:uid="{19175E92-A865-43FC-B974-6C70704F53F3}"/>
-    <hyperlink ref="G98" r:id="rId77" xr:uid="{3A425333-5D51-4904-B101-09E29E630F6C}"/>
-    <hyperlink ref="G99" r:id="rId78" xr:uid="{E7A74BF0-AE57-410B-839C-A5D4E43F88AE}"/>
-    <hyperlink ref="G100" r:id="rId79" xr:uid="{E9708E8F-685B-4930-B0A9-25879DAD1F1C}"/>
-    <hyperlink ref="G102" r:id="rId80" xr:uid="{02B981DE-8A76-44DE-810E-DD00E6B83172}"/>
-    <hyperlink ref="G103" r:id="rId81" xr:uid="{D2CF30ED-7D17-47C8-A540-2D8C897B4AE7}"/>
-    <hyperlink ref="G104" r:id="rId82" xr:uid="{CBFD705D-4078-4323-9DE0-245D4CD7F2EA}"/>
-    <hyperlink ref="G105" r:id="rId83" xr:uid="{554C4472-EC10-44EC-8082-9516F1F47373}"/>
-    <hyperlink ref="G106" r:id="rId84" xr:uid="{801C3CD5-AD39-4A61-B801-FE198D8D9162}"/>
-    <hyperlink ref="G108" r:id="rId85" xr:uid="{4CAC1173-D4BB-4C7E-B092-00EC634DFCFF}"/>
-    <hyperlink ref="G110" r:id="rId86" xr:uid="{D80620C9-DA12-41D8-8162-952ACB81A716}"/>
-    <hyperlink ref="G111" r:id="rId87" xr:uid="{7E3451A1-3A19-4B95-B4BC-A64DC97CC3F2}"/>
-    <hyperlink ref="G112" r:id="rId88" xr:uid="{461E39AF-9147-4BA3-A2C0-C9916A9F2712}"/>
-    <hyperlink ref="G113" r:id="rId89" xr:uid="{E12D5B31-C4A2-4E06-A370-2F54671F7863}"/>
-    <hyperlink ref="G114" r:id="rId90" xr:uid="{D77C3835-CF3D-453A-9BA5-E1B24A06FCCF}"/>
-    <hyperlink ref="G115" r:id="rId91" xr:uid="{5569B989-CCAC-4896-8E0F-BA95FB8045AE}"/>
-    <hyperlink ref="G117" r:id="rId92" xr:uid="{61D12E5E-3BEF-48E8-B8C9-5A1EC76137E8}"/>
-    <hyperlink ref="G119" r:id="rId93" xr:uid="{2C8BE2CD-155B-4759-BBAA-07DBC4B3CCE5}"/>
-    <hyperlink ref="G120" r:id="rId94" xr:uid="{8BA3D887-13D1-4CCF-AD3B-657511504136}"/>
-    <hyperlink ref="G121" r:id="rId95" xr:uid="{46B74643-2CEA-4394-9508-AEE816F46169}"/>
-    <hyperlink ref="G122" r:id="rId96" xr:uid="{4B97AAEF-4038-4260-A91F-30AF7387C89F}"/>
-    <hyperlink ref="G123" r:id="rId97" xr:uid="{1E78EF46-2779-4D0A-A856-40358A27C21D}"/>
-    <hyperlink ref="G124" r:id="rId98" xr:uid="{E2955030-0A78-4BFF-9FE0-FEA0C5095280}"/>
-    <hyperlink ref="G125" r:id="rId99" xr:uid="{7AA5194E-8AEE-4350-99AA-A86885F9DF31}"/>
-    <hyperlink ref="G126" r:id="rId100" xr:uid="{0A9E57BB-75C9-4055-BE7D-A05AB75EBB6A}"/>
-    <hyperlink ref="G127" r:id="rId101" xr:uid="{2D6CCF82-1968-47DD-A5E0-8953B6288F10}"/>
-    <hyperlink ref="G128" r:id="rId102" xr:uid="{11F8A74E-360D-44A8-9866-43654CF2E46D}"/>
-    <hyperlink ref="G130" r:id="rId103" xr:uid="{D7668688-6380-4516-B521-8362047D8340}"/>
-    <hyperlink ref="G131" r:id="rId104" xr:uid="{0113DD9D-40F6-4971-8749-518E8AD30EF9}"/>
-    <hyperlink ref="G132" r:id="rId105" xr:uid="{58F24224-7B6E-4F2E-9C59-654CE0E99C05}"/>
-    <hyperlink ref="G133" r:id="rId106" xr:uid="{1C40EEF8-4349-41B1-84EC-700D72A301F5}"/>
-    <hyperlink ref="G134" r:id="rId107" xr:uid="{A44727A8-7EFA-47E8-B32A-E676B304277B}"/>
-    <hyperlink ref="G135" r:id="rId108" xr:uid="{E8E1D2E0-145C-464E-814C-46773D32D8B9}"/>
-    <hyperlink ref="G136" r:id="rId109" xr:uid="{B563FA46-9306-4D15-9013-109D91E92E06}"/>
-    <hyperlink ref="G137" r:id="rId110" xr:uid="{B823582B-EABF-4085-AEA2-F410F1014470}"/>
-    <hyperlink ref="G138" r:id="rId111" xr:uid="{C56FCF5B-D9F0-4B2E-BDFD-49E622BA291A}"/>
-    <hyperlink ref="G139" r:id="rId112" xr:uid="{AF696A65-6F22-4737-90D6-7DBDB43A722A}"/>
-    <hyperlink ref="G140" r:id="rId113" xr:uid="{2C0AF0BB-E8E4-4BE9-B9D0-AD505A4613F5}"/>
-    <hyperlink ref="G141" r:id="rId114" xr:uid="{D1C67CA6-CEB8-4580-9EFD-1DA619719179}"/>
-    <hyperlink ref="G142" r:id="rId115" xr:uid="{6D7C634B-6519-4ADB-8F57-B1EDE24A72FF}"/>
-    <hyperlink ref="G143" r:id="rId116" xr:uid="{1818B936-07B1-4104-8F4F-860971AAC48F}"/>
-    <hyperlink ref="G144" r:id="rId117" xr:uid="{1B9273CC-8019-45F1-A64D-460BC93490E8}"/>
-    <hyperlink ref="G145" r:id="rId118" xr:uid="{36E2DC91-42DA-4BF4-8872-72701031D1BA}"/>
-    <hyperlink ref="G146" r:id="rId119" xr:uid="{578533B0-C9A3-4ED3-9F54-C5E208F10E08}"/>
-    <hyperlink ref="G147" r:id="rId120" xr:uid="{AEF5D25B-5978-476F-9CC5-F877A81E9672}"/>
-    <hyperlink ref="G148" r:id="rId121" xr:uid="{F22C86FD-35A3-4592-8694-967E1A4EDE39}"/>
-    <hyperlink ref="G149" r:id="rId122" xr:uid="{0F5703C4-44B0-4D69-B4FF-BFF3BB63BCED}"/>
-    <hyperlink ref="G150" r:id="rId123" xr:uid="{9FBE8F89-474A-44C7-85DA-21CDA5FFA143}"/>
-    <hyperlink ref="G151" r:id="rId124" xr:uid="{29062811-5673-407D-B38B-D05C7B31C405}"/>
-    <hyperlink ref="G152" r:id="rId125" xr:uid="{7B21D999-1C90-4F51-BFD2-F74832C4899B}"/>
-    <hyperlink ref="G154" r:id="rId126" xr:uid="{F8972EF7-1211-4B4F-A878-85C635A93088}"/>
-    <hyperlink ref="G155" r:id="rId127" xr:uid="{7BC44D40-98BD-4498-821F-1DDFC0AE9B20}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{93A3DA59-A425-42B4-8D5F-58614DBB0F5B}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{6A4E133A-7492-4221-B4CB-1EF3B0AB94D0}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{FFD8CADC-5728-4ABB-9956-70A6F447CC2C}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{D013559B-C157-4E85-9A8C-C6E7B9881BDB}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{5730BF1F-46E4-4897-879A-176A89C130A5}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{4D8B7151-1212-4EBD-A397-486C81979B4C}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{86F66F59-F1D3-4071-BBF0-8010B161B8E5}"/>
+    <hyperlink ref="F11" r:id="rId8" xr:uid="{2D8970E9-447B-42C2-A88D-A2C765B8617D}"/>
+    <hyperlink ref="F13" r:id="rId9" location="building-and-deploying-mrtk-to-hololens-1-and-hololens-2-uwp" xr:uid="{71AF9FF5-8B79-4A5E-94D2-2B30B05E611E}"/>
+    <hyperlink ref="F14" r:id="rId10" xr:uid="{B64CEDE7-5C9A-446A-9344-9AA23CAAF32C}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{8DC6C39F-E9AB-4D54-A755-88A3F4F9CC2E}"/>
+    <hyperlink ref="F16" r:id="rId12" location="finding-the-current-version" xr:uid="{2E9E623A-32DE-464C-9016-6358575FBC7E}"/>
+    <hyperlink ref="F18" r:id="rId13" xr:uid="{D6EB05E2-FF4D-4F2E-8CCF-761BF38C3456}"/>
+    <hyperlink ref="F19" r:id="rId14" xr:uid="{F38F93B5-24D2-4784-8B82-6E1EBBA7881C}"/>
+    <hyperlink ref="F21" r:id="rId15" xr:uid="{ADF6E112-9990-4660-B1A8-FF7BF284742A}"/>
+    <hyperlink ref="F22" r:id="rId16" xr:uid="{49EBDDB4-2E4C-4855-9AE0-FDBD4D801881}"/>
+    <hyperlink ref="F23" r:id="rId17" xr:uid="{11CE312F-0283-4B88-B42B-B489A3793E64}"/>
+    <hyperlink ref="F25" r:id="rId18" xr:uid="{5E5CC973-FB34-4E0D-8465-A736DD70BD69}"/>
+    <hyperlink ref="F26" r:id="rId19" xr:uid="{89E341CC-6F40-4B2C-90FF-F45082C6597F}"/>
+    <hyperlink ref="F28" r:id="rId20" xr:uid="{3854E21E-81F2-4C0D-894F-58CF18910E54}"/>
+    <hyperlink ref="F29" r:id="rId21" xr:uid="{B277221E-CB8C-4ED3-AAAB-DDEA402EA2D8}"/>
+    <hyperlink ref="F30" r:id="rId22" xr:uid="{981DD41E-1D06-4B57-A808-45913634D62E}"/>
+    <hyperlink ref="F31" r:id="rId23" xr:uid="{B337741F-12AB-4AA5-AE43-46FD1313E145}"/>
+    <hyperlink ref="F34" r:id="rId24" xr:uid="{D17E8A7B-5D5D-46D9-BBD6-884A346BE888}"/>
+    <hyperlink ref="F35" r:id="rId25" xr:uid="{4EA77164-7B03-425B-A93C-B54C08184C14}"/>
+    <hyperlink ref="F37" r:id="rId26" xr:uid="{B10F0F97-4FF1-4131-B36D-516E7CBCCC60}"/>
+    <hyperlink ref="F38" r:id="rId27" xr:uid="{07398E30-E603-49F8-85EA-6C026173A549}"/>
+    <hyperlink ref="F39" r:id="rId28" xr:uid="{C8F4A9E4-39F8-42B0-BE8A-796628212166}"/>
+    <hyperlink ref="F40" r:id="rId29" xr:uid="{680D7AAB-C71C-4E05-A455-59970D35D2EF}"/>
+    <hyperlink ref="F42" r:id="rId30" xr:uid="{510B2B6C-F700-4B42-8222-9824F10312AA}"/>
+    <hyperlink ref="F43" r:id="rId31" xr:uid="{A9AE4DED-6750-451F-B2F1-9878F2064B77}"/>
+    <hyperlink ref="F44" r:id="rId32" xr:uid="{97A3FCDE-117F-467B-82EE-49415B13685C}"/>
+    <hyperlink ref="F45" r:id="rId33" xr:uid="{54B09E6C-82C8-4B1B-A90B-EA2189EA7DC1}"/>
+    <hyperlink ref="F47" r:id="rId34" xr:uid="{3F685F22-DEF1-4908-8F14-957B4596873C}"/>
+    <hyperlink ref="F48" r:id="rId35" xr:uid="{8525CEA4-BB37-4962-871B-93BE3F8D8695}"/>
+    <hyperlink ref="F49" r:id="rId36" xr:uid="{99AD427F-01DB-4E95-8AAB-373215FAC669}"/>
+    <hyperlink ref="F51" r:id="rId37" xr:uid="{C41F81C9-8B2A-4BAE-BE13-E0FFE7521B30}"/>
+    <hyperlink ref="F52" r:id="rId38" xr:uid="{7422CF83-A8B3-4972-8898-2E3ECFA7D73B}"/>
+    <hyperlink ref="F53" r:id="rId39" xr:uid="{3281634E-AF79-4C83-8E61-F001F65FBD15}"/>
+    <hyperlink ref="F54" r:id="rId40" xr:uid="{3FF6B46D-5693-483F-9CD2-F6B802552EEB}"/>
+    <hyperlink ref="F56" r:id="rId41" xr:uid="{1FF1D250-458C-41FE-A035-3A1B9E0B6306}"/>
+    <hyperlink ref="F57" r:id="rId42" xr:uid="{4BB4DAA4-48A5-4640-B10F-0CBCD6A3BE12}"/>
+    <hyperlink ref="F58" r:id="rId43" xr:uid="{DB319251-7975-47A0-88CD-66FE8B9D5A62}"/>
+    <hyperlink ref="F59" r:id="rId44" xr:uid="{61A6D1B8-6B13-4B13-8C2C-88D2A085DCB5}"/>
+    <hyperlink ref="F61" r:id="rId45" xr:uid="{A13684DA-A5FB-4215-BF53-D837E5E9C76D}"/>
+    <hyperlink ref="F62" r:id="rId46" xr:uid="{616C1391-EAAB-4EBB-8C50-87D322C11877}"/>
+    <hyperlink ref="F63" r:id="rId47" xr:uid="{449B57F6-DFF2-4AD1-A178-FB6212AF3533}"/>
+    <hyperlink ref="F64" r:id="rId48" xr:uid="{730E491B-25F4-49CA-AD1D-5F5C04A2ADFC}"/>
+    <hyperlink ref="F66" r:id="rId49" xr:uid="{E413D097-57C9-47E5-9B67-6CA9DAC60C2B}"/>
+    <hyperlink ref="F67" r:id="rId50" xr:uid="{B9F69EED-4326-496E-B8AB-9E5072CCD4AC}"/>
+    <hyperlink ref="F68" r:id="rId51" xr:uid="{E8298287-BC71-4C33-8B39-49E93C287430}"/>
+    <hyperlink ref="F69" r:id="rId52" xr:uid="{01C4BCBC-0FAB-4FC0-BB28-ED1413937CC8}"/>
+    <hyperlink ref="F70" r:id="rId53" xr:uid="{4D0370F5-CCC4-4C9D-B5CC-4463BF0B9870}"/>
+    <hyperlink ref="F71" r:id="rId54" xr:uid="{67844097-C438-43EA-B9E0-79595395094B}"/>
+    <hyperlink ref="F72" r:id="rId55" xr:uid="{E3B3DEA8-7B43-4DBD-9942-A48B4BFF60FA}"/>
+    <hyperlink ref="F73" r:id="rId56" xr:uid="{B1446712-A623-43A7-9B4F-69AEB1C02B34}"/>
+    <hyperlink ref="F74" r:id="rId57" xr:uid="{42A7C29B-0D9C-4061-AD34-C34E9E1E5344}"/>
+    <hyperlink ref="F75" r:id="rId58" xr:uid="{3BFB3FB4-DA5C-413D-922F-5358384FBA37}"/>
+    <hyperlink ref="F76" r:id="rId59" xr:uid="{CB67CB8A-E75C-42B9-92A1-B1D711A008A0}"/>
+    <hyperlink ref="F77" r:id="rId60" xr:uid="{BD9A5733-C0BB-4829-95F4-018DD4948471}"/>
+    <hyperlink ref="F78" r:id="rId61" xr:uid="{CB9921CA-A1B1-4C7D-987A-D84886884DE3}"/>
+    <hyperlink ref="F79" r:id="rId62" xr:uid="{325B681B-9A9E-4367-86FD-646A297873A6}"/>
+    <hyperlink ref="F81" r:id="rId63" xr:uid="{7C24BD78-580C-4B83-92CE-4F9A73DF21D1}"/>
+    <hyperlink ref="F82" r:id="rId64" xr:uid="{837FE256-264A-48D1-B4A0-3DC9D41F01D7}"/>
+    <hyperlink ref="F83" r:id="rId65" xr:uid="{0F2B7185-552E-4967-83AC-A300D874A411}"/>
+    <hyperlink ref="F84" r:id="rId66" xr:uid="{3CD22473-AE2E-4B8D-AA0C-DA1A3FD73D3D}"/>
+    <hyperlink ref="F85" r:id="rId67" xr:uid="{464AA96C-2E81-4DD8-971E-FB5A8F22FE54}"/>
+    <hyperlink ref="F86" r:id="rId68" xr:uid="{45CE71C8-7B3B-4152-8E12-920A52C953B8}"/>
+    <hyperlink ref="F87" r:id="rId69" xr:uid="{523C8272-EA14-44CF-9A75-0B5E9776BD07}"/>
+    <hyperlink ref="F89" r:id="rId70" xr:uid="{1A1116FD-CD0C-4E49-88D6-DA7B8E263BC8}"/>
+    <hyperlink ref="F90" r:id="rId71" xr:uid="{81E073F9-AEDE-45AC-A164-27B3119B458B}"/>
+    <hyperlink ref="F91" r:id="rId72" xr:uid="{6F138136-5044-4F83-91EB-B24E0D69A3E0}"/>
+    <hyperlink ref="F93" r:id="rId73" xr:uid="{391F87F3-211E-4A04-B158-DEEBE023F73F}"/>
+    <hyperlink ref="F95" r:id="rId74" xr:uid="{719FAA48-4EC4-4D08-B666-9E72202F5A08}"/>
+    <hyperlink ref="F96" r:id="rId75" xr:uid="{B99681F4-0AC8-4290-B61A-32C580BE0E3E}"/>
+    <hyperlink ref="F97" r:id="rId76" xr:uid="{19175E92-A865-43FC-B974-6C70704F53F3}"/>
+    <hyperlink ref="F98" r:id="rId77" xr:uid="{3A425333-5D51-4904-B101-09E29E630F6C}"/>
+    <hyperlink ref="F99" r:id="rId78" xr:uid="{E7A74BF0-AE57-410B-839C-A5D4E43F88AE}"/>
+    <hyperlink ref="F100" r:id="rId79" xr:uid="{E9708E8F-685B-4930-B0A9-25879DAD1F1C}"/>
+    <hyperlink ref="F102" r:id="rId80" xr:uid="{02B981DE-8A76-44DE-810E-DD00E6B83172}"/>
+    <hyperlink ref="F103" r:id="rId81" xr:uid="{D2CF30ED-7D17-47C8-A540-2D8C897B4AE7}"/>
+    <hyperlink ref="F104" r:id="rId82" xr:uid="{CBFD705D-4078-4323-9DE0-245D4CD7F2EA}"/>
+    <hyperlink ref="F105" r:id="rId83" xr:uid="{554C4472-EC10-44EC-8082-9516F1F47373}"/>
+    <hyperlink ref="F106" r:id="rId84" xr:uid="{801C3CD5-AD39-4A61-B801-FE198D8D9162}"/>
+    <hyperlink ref="F108" r:id="rId85" xr:uid="{4CAC1173-D4BB-4C7E-B092-00EC634DFCFF}"/>
+    <hyperlink ref="F110" r:id="rId86" xr:uid="{D80620C9-DA12-41D8-8162-952ACB81A716}"/>
+    <hyperlink ref="F111" r:id="rId87" xr:uid="{7E3451A1-3A19-4B95-B4BC-A64DC97CC3F2}"/>
+    <hyperlink ref="F112" r:id="rId88" xr:uid="{461E39AF-9147-4BA3-A2C0-C9916A9F2712}"/>
+    <hyperlink ref="F113" r:id="rId89" xr:uid="{E12D5B31-C4A2-4E06-A370-2F54671F7863}"/>
+    <hyperlink ref="F114" r:id="rId90" xr:uid="{D77C3835-CF3D-453A-9BA5-E1B24A06FCCF}"/>
+    <hyperlink ref="F115" r:id="rId91" xr:uid="{5569B989-CCAC-4896-8E0F-BA95FB8045AE}"/>
+    <hyperlink ref="F117" r:id="rId92" xr:uid="{61D12E5E-3BEF-48E8-B8C9-5A1EC76137E8}"/>
+    <hyperlink ref="F119" r:id="rId93" xr:uid="{2C8BE2CD-155B-4759-BBAA-07DBC4B3CCE5}"/>
+    <hyperlink ref="F120" r:id="rId94" xr:uid="{8BA3D887-13D1-4CCF-AD3B-657511504136}"/>
+    <hyperlink ref="F121" r:id="rId95" xr:uid="{46B74643-2CEA-4394-9508-AEE816F46169}"/>
+    <hyperlink ref="F122" r:id="rId96" xr:uid="{4B97AAEF-4038-4260-A91F-30AF7387C89F}"/>
+    <hyperlink ref="F123" r:id="rId97" xr:uid="{1E78EF46-2779-4D0A-A856-40358A27C21D}"/>
+    <hyperlink ref="F124" r:id="rId98" xr:uid="{E2955030-0A78-4BFF-9FE0-FEA0C5095280}"/>
+    <hyperlink ref="F125" r:id="rId99" xr:uid="{7AA5194E-8AEE-4350-99AA-A86885F9DF31}"/>
+    <hyperlink ref="F126" r:id="rId100" xr:uid="{0A9E57BB-75C9-4055-BE7D-A05AB75EBB6A}"/>
+    <hyperlink ref="F127" r:id="rId101" xr:uid="{2D6CCF82-1968-47DD-A5E0-8953B6288F10}"/>
+    <hyperlink ref="F128" r:id="rId102" xr:uid="{11F8A74E-360D-44A8-9866-43654CF2E46D}"/>
+    <hyperlink ref="F130" r:id="rId103" xr:uid="{D7668688-6380-4516-B521-8362047D8340}"/>
+    <hyperlink ref="F131" r:id="rId104" xr:uid="{0113DD9D-40F6-4971-8749-518E8AD30EF9}"/>
+    <hyperlink ref="F132" r:id="rId105" xr:uid="{58F24224-7B6E-4F2E-9C59-654CE0E99C05}"/>
+    <hyperlink ref="F133" r:id="rId106" xr:uid="{1C40EEF8-4349-41B1-84EC-700D72A301F5}"/>
+    <hyperlink ref="F134" r:id="rId107" xr:uid="{A44727A8-7EFA-47E8-B32A-E676B304277B}"/>
+    <hyperlink ref="F135" r:id="rId108" xr:uid="{E8E1D2E0-145C-464E-814C-46773D32D8B9}"/>
+    <hyperlink ref="F136" r:id="rId109" xr:uid="{B563FA46-9306-4D15-9013-109D91E92E06}"/>
+    <hyperlink ref="F137" r:id="rId110" xr:uid="{B823582B-EABF-4085-AEA2-F410F1014470}"/>
+    <hyperlink ref="F138" r:id="rId111" xr:uid="{C56FCF5B-D9F0-4B2E-BDFD-49E622BA291A}"/>
+    <hyperlink ref="F139" r:id="rId112" xr:uid="{AF696A65-6F22-4737-90D6-7DBDB43A722A}"/>
+    <hyperlink ref="F140" r:id="rId113" xr:uid="{2C0AF0BB-E8E4-4BE9-B9D0-AD505A4613F5}"/>
+    <hyperlink ref="F141" r:id="rId114" xr:uid="{D1C67CA6-CEB8-4580-9EFD-1DA619719179}"/>
+    <hyperlink ref="F142" r:id="rId115" xr:uid="{6D7C634B-6519-4ADB-8F57-B1EDE24A72FF}"/>
+    <hyperlink ref="F143" r:id="rId116" xr:uid="{1818B936-07B1-4104-8F4F-860971AAC48F}"/>
+    <hyperlink ref="F144" r:id="rId117" xr:uid="{1B9273CC-8019-45F1-A64D-460BC93490E8}"/>
+    <hyperlink ref="F145" r:id="rId118" xr:uid="{36E2DC91-42DA-4BF4-8872-72701031D1BA}"/>
+    <hyperlink ref="F146" r:id="rId119" xr:uid="{578533B0-C9A3-4ED3-9F54-C5E208F10E08}"/>
+    <hyperlink ref="F147" r:id="rId120" xr:uid="{AEF5D25B-5978-476F-9CC5-F877A81E9672}"/>
+    <hyperlink ref="F148" r:id="rId121" xr:uid="{F22C86FD-35A3-4592-8694-967E1A4EDE39}"/>
+    <hyperlink ref="F149" r:id="rId122" xr:uid="{0F5703C4-44B0-4D69-B4FF-BFF3BB63BCED}"/>
+    <hyperlink ref="F150" r:id="rId123" xr:uid="{9FBE8F89-474A-44C7-85DA-21CDA5FFA143}"/>
+    <hyperlink ref="F151" r:id="rId124" xr:uid="{29062811-5673-407D-B38B-D05C7B31C405}"/>
+    <hyperlink ref="F152" r:id="rId125" xr:uid="{7B21D999-1C90-4F51-BFD2-F74832C4899B}"/>
+    <hyperlink ref="F154" r:id="rId126" xr:uid="{F8972EF7-1211-4B4F-A878-85C635A93088}"/>
+    <hyperlink ref="F155" r:id="rId127" xr:uid="{7BC44D40-98BD-4498-821F-1DDFC0AE9B20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>